<commit_message>
Enable exceedance and time series SHArea analysis
</commit_message>
<xml_diff>
--- a/00_Flows/templates/flow_return_period_template.xlsx
+++ b/00_Flows/templates/flow_return_period_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\RiverArchitect\.site_packages\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\RiverArchitect\00_Flows\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
+    <t>SET UNIT SYSTEM:</t>
+  </si>
+  <si>
+    <t>U.S. customary</t>
+  </si>
+  <si>
     <t>Discharge</t>
+  </si>
+  <si>
+    <t>Return period</t>
   </si>
   <si>
     <t>Associated depth raster</t>
@@ -31,34 +40,24 @@
     <t>Associated velocity raster</t>
   </si>
   <si>
+    <t>(years)</t>
+  </si>
+  <si>
     <t>(filename)</t>
   </si>
   <si>
     <t>units</t>
   </si>
   <si>
-    <t>U.S. customary</t>
-  </si>
-  <si>
     <t>SI (metric)</t>
-  </si>
-  <si>
-    <t>Return period</t>
-  </si>
-  <si>
-    <t>(years)</t>
-  </si>
-  <si>
-    <t>SET UNIT SYSTEM:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -121,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -168,12 +167,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,10 +212,13 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -212,53 +227,41 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial Narrow"/>
-        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial Narrow"/>
-        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial Narrow"/>
-        <scheme val="none"/>
       </font>
     </dxf>
   </dxfs>
@@ -288,9 +291,23 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5258140539520406E-2"/>
+          <c:y val="3.8357483056941394E-2"/>
+          <c:w val="0.86925713467330601"/>
+          <c:h val="0.80630245729732797"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -299,12 +316,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>flows!$C$3</c:f>
+              <c:f>flows!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Return period</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -338,7 +352,7 @@
             <c:numRef>
               <c:f>flows!$C$5:$C$201</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="197"/>
               </c:numCache>
             </c:numRef>
@@ -355,7 +369,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B150-4C74-866A-CF7B735459BA}"/>
+              <c16:uniqueId val="{00000000-1452-4AD3-A095-DA2A2AFC0E58}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -374,6 +388,7 @@
         <c:axId val="1334583648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -517,8 +532,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.7326430356145572E-2"/>
-              <c:y val="0.38317827479801386"/>
+              <c:x val="1.9451264175736806E-2"/>
+              <c:y val="0.30279386062316771"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -888,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E200"/>
+  <dimension ref="B1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -901,683 +916,207 @@
     <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="6" width="9.140625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="11" t="s">
-        <v>9</v>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="str">
-        <f xml:space="preserve"> IF($D$1="U.S. customary", "(cfs)", "(m³/s)")</f>
+        <f>IF($D$1="U.S. customary", "(cfs)", "(m³/s)")</f>
         <v>(cfs)</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="10"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="10"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="10"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="10"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="10"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="10"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="10"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="10"/>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="10"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="10"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="10"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C53" s="10"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C55" s="10"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C59" s="10"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C61" s="10"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C62" s="10"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C63" s="10"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C65" s="10"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C67" s="10"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C69" s="10"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C71" s="10"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C72" s="10"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C73" s="10"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C74" s="10"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C75" s="10"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C76" s="10"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C77" s="10"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C78" s="10"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C79" s="10"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C81" s="10"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C83" s="10"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C84" s="10"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C85" s="10"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C87" s="10"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C89" s="10"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C91" s="10"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C92" s="10"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C93" s="10"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C94" s="10"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C95" s="10"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C96" s="10"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C97" s="10"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C99" s="10"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C100" s="10"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C101" s="10"/>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C102" s="10"/>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C103" s="10"/>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C104" s="10"/>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C105" s="10"/>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C106" s="10"/>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C107" s="10"/>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C108" s="10"/>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C109" s="10"/>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C110" s="10"/>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C111" s="10"/>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C112" s="10"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C113" s="10"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C114" s="10"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C115" s="10"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C116" s="10"/>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C117" s="10"/>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C118" s="10"/>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C119" s="10"/>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C120" s="10"/>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C121" s="10"/>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C122" s="10"/>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C123" s="10"/>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C124" s="10"/>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C125" s="10"/>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C126" s="10"/>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C127" s="10"/>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C128" s="10"/>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C129" s="10"/>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C130" s="10"/>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C131" s="10"/>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C132" s="10"/>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C133" s="10"/>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C134" s="10"/>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C135" s="10"/>
-    </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C136" s="10"/>
-    </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C137" s="10"/>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C138" s="10"/>
-    </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C139" s="10"/>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C140" s="10"/>
-    </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C141" s="10"/>
-    </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C142" s="10"/>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C143" s="10"/>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C144" s="10"/>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C145" s="10"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C146" s="10"/>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C147" s="10"/>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C148" s="10"/>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C149" s="10"/>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C150" s="10"/>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C151" s="10"/>
-    </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C152" s="10"/>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C153" s="10"/>
-    </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C154" s="10"/>
-    </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C155" s="10"/>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C156" s="10"/>
-    </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C157" s="10"/>
-    </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C158" s="10"/>
-    </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C159" s="10"/>
-    </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C160" s="10"/>
-    </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C161" s="10"/>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C162" s="10"/>
-    </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C163" s="10"/>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C164" s="10"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C165" s="10"/>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C166" s="10"/>
-    </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C167" s="10"/>
-    </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C168" s="10"/>
-    </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C169" s="10"/>
-    </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C170" s="10"/>
-    </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C171" s="10"/>
-    </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C172" s="10"/>
-    </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C173" s="10"/>
-    </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C174" s="10"/>
-    </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C175" s="10"/>
-    </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C176" s="10"/>
-    </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C177" s="10"/>
-    </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C178" s="10"/>
-    </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C179" s="10"/>
-    </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C180" s="10"/>
-    </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C181" s="10"/>
-    </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C182" s="10"/>
-    </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C183" s="10"/>
-    </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C184" s="10"/>
-    </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C185" s="10"/>
-    </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C186" s="10"/>
-    </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C187" s="10"/>
-    </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C188" s="10"/>
-    </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C189" s="10"/>
-    </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C190" s="10"/>
-    </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C191" s="10"/>
-    </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C192" s="10"/>
-    </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C193" s="10"/>
-    </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C194" s="10"/>
-    </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C195" s="10"/>
-    </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C196" s="10"/>
-    </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C197" s="10"/>
-    </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C198" s="10"/>
-    </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C199" s="10"/>
-    </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C200" s="10"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="8"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="8"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="8"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="8"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="8"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="8"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'.templates'!$B$3:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1591,31 +1130,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="9.140625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>